<commit_message>
Atualizacao de Adicao de Links
Commit autorizado pelo professor para adicionar links nas planilhas
desatualizadas
</commit_message>
<xml_diff>
--- a/Entregavel_02/Sprint_03/GQA/GQA-CHQ-CHECKLIST_DE_QUALIDADE.xlsx
+++ b/Entregavel_02/Sprint_03/GQA/GQA-CHQ-CHECKLIST_DE_QUALIDADE.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instruções" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,12 @@
     <sheet name="GCO" sheetId="4" r:id="rId4"/>
     <sheet name="Resultados" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="104">
   <si>
     <t>Cada pergunta é respondida com:</t>
   </si>
@@ -128,9 +128,6 @@
     <t>Foram identificados os produtos que deverão ser entregues no final do projeto? </t>
   </si>
   <si>
-    <t>As atividades que estão no plano de projeto, mais que não serão contempladas no projeto, foram listadas e o motivo foi explicado? </t>
-  </si>
-  <si>
     <t>As priorizações das tarefas foram consideradas nas alocações nos ciclos de desenvolvimento? </t>
   </si>
   <si>
@@ -270,13 +267,76 @@
   </si>
   <si>
     <t xml:space="preserve"> Plano de Projeto - Sessao 8 - Sessao 2 - Sessao 9</t>
+  </si>
+  <si>
+    <t>Plano de Gerência de Configuração - Sessão 9</t>
+  </si>
+  <si>
+    <t>Plano de Projeto - Sessão 4 - Sessão 3 Análise de Viabilidade</t>
+  </si>
+  <si>
+    <t>Plano de Projeto - Sessão 5 Aprovação</t>
+  </si>
+  <si>
+    <t>Plano de Projeto - Sessão 2 Marcos e Ponto de Controle</t>
+  </si>
+  <si>
+    <t>Relatório de Acompanhamento do Projeto - Sessão 2</t>
+  </si>
+  <si>
+    <t>Relatório de Acompanhamento do Projeto - Sessão 1 Atividades - Sessão 1 Avaliação da Equipe</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Cronogramas e Atividades Detalhadas - Sessão 3</t>
+  </si>
+  <si>
+    <t>Gerenciamento de Riscos - Sessão 2</t>
+  </si>
+  <si>
+    <t>Método de Estimativa</t>
+  </si>
+  <si>
+    <t>Plano de Projeto</t>
+  </si>
+  <si>
+    <t>As atividades que estão no plano de projeto, mas que não serão contempladas no projeto, foram listadas e o motivo foi explicado? </t>
+  </si>
+  <si>
+    <t>Checklist Acompanhamento de Requisitos</t>
+  </si>
+  <si>
+    <t>Aprovação dos Requisitos</t>
+  </si>
+  <si>
+    <t>Solicitação de Aprovação</t>
+  </si>
+  <si>
+    <t>Acompanhamento de Requisitos</t>
+  </si>
+  <si>
+    <t>Mudança de Requisito</t>
+  </si>
+  <si>
+    <t>Processo de Gerência de Requisitos</t>
+  </si>
+  <si>
+    <t>Especificação de Requisitos Final</t>
+  </si>
+  <si>
+    <t>Relatório de Requisitos e Formalidades - Sessão 2</t>
+  </si>
+  <si>
+    <t>Relatório de Requisitos e Formalidades</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -338,6 +398,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -543,7 +609,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -602,9 +668,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -644,6 +707,16 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -942,11 +1015,11 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -1199,8 +1272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
@@ -1238,8 +1311,8 @@
       <c r="C2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="50" t="s">
-        <v>81</v>
+      <c r="D2" s="49" t="s">
+        <v>80</v>
       </c>
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
@@ -1254,8 +1327,8 @@
       <c r="C3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="50" t="s">
-        <v>82</v>
+      <c r="D3" s="49" t="s">
+        <v>81</v>
       </c>
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
@@ -1268,10 +1341,10 @@
         <v>28</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" s="50" t="s">
-        <v>83</v>
+        <v>79</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>82</v>
       </c>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
@@ -1286,7 +1359,9 @@
       <c r="C5" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="22"/>
+      <c r="D5" s="49" t="s">
+        <v>83</v>
+      </c>
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
     </row>
@@ -1300,7 +1375,9 @@
       <c r="C6" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="22"/>
+      <c r="D6" s="49" t="s">
+        <v>84</v>
+      </c>
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
     </row>
@@ -1314,7 +1391,9 @@
       <c r="C7" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
+      <c r="D7" s="49" t="s">
+        <v>87</v>
+      </c>
       <c r="E7" s="18"/>
       <c r="F7" s="18"/>
     </row>
@@ -1328,7 +1407,9 @@
       <c r="C8" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="22"/>
+      <c r="D8" s="49" t="s">
+        <v>85</v>
+      </c>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
     </row>
@@ -1342,7 +1423,9 @@
       <c r="C9" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="22"/>
+      <c r="D9" s="49" t="s">
+        <v>86</v>
+      </c>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
     </row>
@@ -1356,7 +1439,9 @@
       <c r="C10" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="22"/>
+      <c r="D10" s="49" t="s">
+        <v>88</v>
+      </c>
       <c r="E10" s="18"/>
       <c r="F10" s="18"/>
     </row>
@@ -1370,7 +1455,9 @@
       <c r="C11" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="22"/>
+      <c r="D11" s="49" t="s">
+        <v>89</v>
+      </c>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
     </row>
@@ -1378,8 +1465,8 @@
       <c r="A12" s="19">
         <v>11</v>
       </c>
-      <c r="B12" s="20" t="s">
-        <v>36</v>
+      <c r="B12" s="30" t="s">
+        <v>94</v>
       </c>
       <c r="C12" s="23" t="s">
         <v>1</v>
@@ -1393,12 +1480,14 @@
         <v>12</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="22"/>
+      <c r="D13" s="49" t="s">
+        <v>90</v>
+      </c>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
     </row>
@@ -1407,12 +1496,14 @@
         <v>13</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="22"/>
+      <c r="D14" s="49" t="s">
+        <v>90</v>
+      </c>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
     </row>
@@ -1421,7 +1512,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="23" t="s">
         <v>1</v>
@@ -1435,7 +1526,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" s="23" t="s">
         <v>1</v>
@@ -1449,12 +1540,14 @@
         <v>17</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="22"/>
+      <c r="D17" s="49" t="s">
+        <v>91</v>
+      </c>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
     </row>
@@ -1463,7 +1556,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" s="23" t="s">
         <v>1</v>
@@ -1477,12 +1570,14 @@
         <v>19</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C19" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="22"/>
+      <c r="D19" s="49" t="s">
+        <v>93</v>
+      </c>
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
     </row>
@@ -1491,7 +1586,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C20" s="23" t="s">
         <v>1</v>
@@ -1505,12 +1600,14 @@
         <v>21</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C21" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="22"/>
+      <c r="D21" s="49" t="s">
+        <v>85</v>
+      </c>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
     </row>
@@ -1519,12 +1616,14 @@
         <v>22</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="22"/>
+      <c r="D22" s="49" t="s">
+        <v>92</v>
+      </c>
       <c r="E22" s="18"/>
       <c r="F22" s="18"/>
     </row>
@@ -1541,8 +1640,22 @@
     <hyperlink ref="D2" r:id="rId1"/>
     <hyperlink ref="D3" r:id="rId2" display=" Plano de Projeto - Sessao 1"/>
     <hyperlink ref="D4" r:id="rId3" display=" Plano de Projeto - Sessao 1"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
+    <hyperlink ref="D8" r:id="rId7"/>
+    <hyperlink ref="D9" r:id="rId8"/>
+    <hyperlink ref="D10" r:id="rId9"/>
+    <hyperlink ref="D11" r:id="rId10"/>
+    <hyperlink ref="D13" r:id="rId11"/>
+    <hyperlink ref="D14" r:id="rId12"/>
+    <hyperlink ref="D17" r:id="rId13"/>
+    <hyperlink ref="D22" r:id="rId14"/>
+    <hyperlink ref="D21" r:id="rId15"/>
+    <hyperlink ref="D19" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId17"/>
 </worksheet>
 </file>
 
@@ -1550,8 +1663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
@@ -1559,7 +1672,7 @@
     <col min="1" max="1" width="5.85546875" customWidth="1"/>
     <col min="2" max="2" width="43.42578125" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="4" max="4" width="56.42578125" customWidth="1"/>
     <col min="5" max="6" width="8" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1584,12 +1697,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="30"/>
+      <c r="D2" s="51" t="s">
+        <v>102</v>
+      </c>
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
     </row>
@@ -1597,13 +1712,15 @@
       <c r="A3" s="28">
         <v>2</v>
       </c>
-      <c r="B3" s="31" t="s">
-        <v>48</v>
+      <c r="B3" s="30" t="s">
+        <v>47</v>
       </c>
       <c r="C3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="32"/>
+      <c r="D3" s="50" t="s">
+        <v>97</v>
+      </c>
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
     </row>
@@ -1612,12 +1729,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="32"/>
+      <c r="D4" s="53" t="s">
+        <v>96</v>
+      </c>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
     </row>
@@ -1626,12 +1745,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="32"/>
+      <c r="D5" s="50" t="s">
+        <v>96</v>
+      </c>
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
     </row>
@@ -1640,12 +1761,12 @@
         <v>5</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="32"/>
+      <c r="D6" s="31"/>
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
     </row>
@@ -1654,12 +1775,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="32"/>
+      <c r="D7" s="50" t="s">
+        <v>101</v>
+      </c>
       <c r="E7" s="18"/>
       <c r="F7" s="18"/>
     </row>
@@ -1668,12 +1791,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="32"/>
+      <c r="D8" s="50" t="s">
+        <v>98</v>
+      </c>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
     </row>
@@ -1682,12 +1807,12 @@
         <v>8</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="32"/>
+      <c r="D9" s="31"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
     </row>
@@ -1696,13 +1821,15 @@
         <v>9</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C10" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="30"/>
-      <c r="E10" s="33"/>
+      <c r="D10" s="51" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="32"/>
       <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:6" ht="75" customHeight="1">
@@ -1710,12 +1837,14 @@
         <v>10</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="30"/>
+      <c r="D11" s="51" t="s">
+        <v>103</v>
+      </c>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
     </row>
@@ -1724,12 +1853,12 @@
         <v>11</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="32"/>
+      <c r="D12" s="52"/>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
     </row>
@@ -1738,12 +1867,14 @@
         <v>12</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="32"/>
+      <c r="D13" s="50" t="s">
+        <v>100</v>
+      </c>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
     </row>
@@ -1752,64 +1883,78 @@
         <v>13</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C14" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="32"/>
+      <c r="D14" s="50" t="s">
+        <v>95</v>
+      </c>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="34"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="35"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="34"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="34"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="35"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="34"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="34"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="35"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="34"/>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="34"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="35"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="34"/>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="34"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="35"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="34"/>
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="34"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="35"/>
+      <c r="A20" s="33"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="34"/>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D14" r:id="rId1"/>
+    <hyperlink ref="D5" r:id="rId2"/>
+    <hyperlink ref="D3" r:id="rId3"/>
+    <hyperlink ref="D8" r:id="rId4"/>
+    <hyperlink ref="D10" r:id="rId5"/>
+    <hyperlink ref="D13" r:id="rId6"/>
+    <hyperlink ref="D7" r:id="rId7"/>
+    <hyperlink ref="D2" r:id="rId8"/>
+    <hyperlink ref="D11" r:id="rId9"/>
+    <hyperlink ref="D4" r:id="rId10"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -1850,196 +1995,196 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="36"/>
+      <c r="D2" s="35"/>
     </row>
     <row r="3" spans="1:4" ht="37.5" customHeight="1">
       <c r="A3" s="28">
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="36"/>
+      <c r="D3" s="35"/>
     </row>
     <row r="4" spans="1:4" ht="37.5" customHeight="1">
       <c r="A4" s="28">
         <v>3</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="36"/>
+      <c r="D4" s="35"/>
     </row>
     <row r="5" spans="1:4" ht="37.5" customHeight="1">
       <c r="A5" s="28">
         <v>4</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="36"/>
+      <c r="D5" s="35"/>
     </row>
     <row r="6" spans="1:4" ht="56.25" customHeight="1">
       <c r="A6" s="28">
         <v>5</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="36"/>
+      <c r="D6" s="35"/>
     </row>
     <row r="7" spans="1:4" ht="37.5" customHeight="1">
       <c r="A7" s="28">
         <v>6</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="36"/>
+      <c r="D7" s="35"/>
     </row>
     <row r="8" spans="1:4" ht="56.25" customHeight="1">
       <c r="A8" s="28">
         <v>7</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="36"/>
+      <c r="D8" s="35"/>
     </row>
     <row r="9" spans="1:4" ht="37.5" customHeight="1">
       <c r="A9" s="28">
         <v>8</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="36"/>
+      <c r="D9" s="35"/>
     </row>
     <row r="10" spans="1:4" ht="37.5" customHeight="1">
       <c r="A10" s="28">
         <v>9</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C10" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="36"/>
+      <c r="D10" s="35"/>
     </row>
     <row r="11" spans="1:4" ht="75" customHeight="1">
       <c r="A11" s="28">
         <v>10</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="36"/>
+        <v>67</v>
+      </c>
+      <c r="C11" s="36"/>
+      <c r="D11" s="35"/>
     </row>
     <row r="12" spans="1:4" ht="75" customHeight="1">
       <c r="A12" s="28">
         <v>11</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="50"/>
+      <c r="D12" s="49"/>
     </row>
     <row r="13" spans="1:4" ht="56.25" customHeight="1">
       <c r="A13" s="28">
         <v>12</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="36"/>
+      <c r="D13" s="35"/>
     </row>
     <row r="14" spans="1:4" ht="37.5" customHeight="1">
       <c r="A14" s="28">
         <v>13</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C14" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="36"/>
+      <c r="D14" s="35"/>
     </row>
     <row r="15" spans="1:4" ht="56.25" customHeight="1">
       <c r="A15" s="28">
         <v>14</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C15" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="36"/>
+      <c r="D15" s="35"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="38"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="41"/>
+      <c r="A16" s="37"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="40"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="38"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="41"/>
+      <c r="A17" s="37"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="40"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="38"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="41"/>
+      <c r="A18" s="37"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="40"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="38"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="41"/>
+      <c r="A19" s="37"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="40"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="38"/>
-      <c r="B20" s="39"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="41"/>
+      <c r="A20" s="37"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -2065,166 +2210,166 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="42"/>
-      <c r="B1" s="42" t="s">
+      <c r="A1" s="41"/>
+      <c r="B1" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="D1" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="E1" s="43" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="44" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="42" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" s="45">
+      <c r="B2" s="44">
         <f>COUNTIFS(GPR!C2:C22,"&lt;&gt;NÃO",GPR!C2:C22,"&lt;&gt;")</f>
         <v>21</v>
       </c>
-      <c r="C2" s="45">
+      <c r="C2" s="44">
         <f>COUNTIF(GPR!A2:A22,"&lt;&gt;")</f>
         <v>21</v>
       </c>
-      <c r="D2" s="46">
+      <c r="D2" s="45">
         <f t="shared" ref="D2:D4" si="0">(B2/C2)</f>
         <v>1</v>
       </c>
-      <c r="E2" s="45" t="str">
+      <c r="E2" s="44" t="str">
         <f t="shared" ref="E2:E4" si="1">IF(D2&lt;=70%,"CRÍTICO",IF(D2&gt;=80%,"NORMAL","ALERTA"))</f>
         <v>NORMAL</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="42" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" s="47">
+      <c r="A3" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="46">
         <f>COUNTIFS(GRE!C2:C14,"&lt;&gt;NÃO",GRE!C2:C14,"&lt;&gt;")</f>
         <v>13</v>
       </c>
-      <c r="C3" s="47">
+      <c r="C3" s="46">
         <f>COUNTIF(GRE!A2:A14,"&lt;&gt;")</f>
         <v>13</v>
       </c>
-      <c r="D3" s="48">
+      <c r="D3" s="47">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E3" s="45" t="str">
+      <c r="E3" s="44" t="str">
         <f t="shared" si="1"/>
         <v>NORMAL</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" s="45">
+      <c r="A4" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="44">
         <f>COUNTIFS(GCO!C2:C15,"&lt;&gt;NÃO",GCO!C2:C15,"&lt;&gt;")</f>
         <v>13</v>
       </c>
-      <c r="C4" s="45">
+      <c r="C4" s="44">
         <f>COUNTIF(GCO!A2:A15,"&lt;&gt;")</f>
         <v>14</v>
       </c>
-      <c r="D4" s="46">
+      <c r="D4" s="45">
         <f t="shared" si="0"/>
         <v>0.9285714285714286</v>
       </c>
-      <c r="E4" s="45" t="str">
+      <c r="E4" s="44" t="str">
         <f t="shared" si="1"/>
         <v>NORMAL</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="41"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="40"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="41"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="40"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="41"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="40"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="41"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="40"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="41"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="40"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="41"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="40"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="41"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="40"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="41"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="40"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="41"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="40"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="41"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="40"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="41"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="40"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="41"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="40"/>
     </row>
     <row r="17" spans="2:5">
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="41"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="40"/>
     </row>
     <row r="18" spans="2:5">
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="41"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>